<commit_message>
edit code and plots
</commit_message>
<xml_diff>
--- a/tracking_data/active_tracking_points.xlsx
+++ b/tracking_data/active_tracking_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindseylabrie/Documents/GitHub/telemetry/tracking_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40950B6-0F1E-E649-895A-EA7952AC36BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F42B64C-1097-8045-9FCA-8D6448D24DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23320" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>10:25:58.208</t>
   </si>
@@ -161,6 +161,33 @@
   </si>
   <si>
     <t>12:08:11.964</t>
+  </si>
+  <si>
+    <t>13:41:17.710</t>
+  </si>
+  <si>
+    <t>14:47:03.662</t>
+  </si>
+  <si>
+    <t>13:49:19.752</t>
+  </si>
+  <si>
+    <t>12:17:07.717</t>
+  </si>
+  <si>
+    <t>11:03:27.276</t>
+  </si>
+  <si>
+    <t>13:29:18.425</t>
+  </si>
+  <si>
+    <t>11:14:44.010</t>
+  </si>
+  <si>
+    <t>12:46:04.002</t>
+  </si>
+  <si>
+    <t>11:42:11.270</t>
   </si>
 </sst>
 </file>
@@ -670,7 +697,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -682,6 +709,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1037,11 +1069,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2240,31 +2272,265 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+    <row r="48" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
         <v>44692</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="11">
         <v>48483</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="12">
         <v>55</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="11">
         <v>42.898980000000002</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="11">
         <v>-97.279139999999998</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="10">
         <v>3.7</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="13">
+        <v>44699</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="1">
+        <v>48468</v>
+      </c>
+      <c r="D49" s="1">
+        <v>79</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>43.068579999999997</v>
+      </c>
+      <c r="G49" s="1">
+        <v>-97.427859999999995</v>
+      </c>
+      <c r="H49" s="8">
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="13">
+        <v>44697</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1">
+        <v>48462</v>
+      </c>
+      <c r="D50" s="1">
+        <v>75</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>43.139249999999997</v>
+      </c>
+      <c r="G50" s="1">
+        <v>-97.536180000000002</v>
+      </c>
+      <c r="H50" s="7">
+        <v>88.85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="13">
+        <v>44697</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="1">
+        <v>48464</v>
+      </c>
+      <c r="D51" s="1">
+        <v>82</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>43.149079999999998</v>
+      </c>
+      <c r="G51" s="1">
+        <v>-97.59563</v>
+      </c>
+      <c r="H51" s="8">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
+        <v>44697</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="12">
+        <v>48478</v>
+      </c>
+      <c r="D52" s="12">
+        <v>74</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>43.19023</v>
+      </c>
+      <c r="G52" s="12">
+        <v>-97.646609999999995</v>
+      </c>
+      <c r="H52" s="10">
+        <v>107.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="14">
+        <v>44707</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="1">
+        <v>48732</v>
+      </c>
+      <c r="D53" s="1">
+        <v>81</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>43.01417</v>
+      </c>
+      <c r="G53" s="1">
+        <v>-97.365530000000007</v>
+      </c>
+      <c r="H53" s="8">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="14">
+        <v>44704</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="1">
+        <v>48462</v>
+      </c>
+      <c r="D54" s="1">
+        <v>76</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>43.139290000000003</v>
+      </c>
+      <c r="G54" s="1">
+        <v>-97.537989999999994</v>
+      </c>
+      <c r="H54" s="8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="15">
+        <v>44704</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="12">
+        <v>48478</v>
+      </c>
+      <c r="D55" s="12">
+        <v>66</v>
+      </c>
+      <c r="E55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="12">
+        <v>43.190510000000003</v>
+      </c>
+      <c r="G55" s="12">
+        <v>-97.647400000000005</v>
+      </c>
+      <c r="H55" s="10">
+        <v>107.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="14">
+        <v>44712</v>
+      </c>
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56">
+        <v>48462</v>
+      </c>
+      <c r="D56">
+        <v>60</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>43.241079999999997</v>
+      </c>
+      <c r="G56">
+        <v>-97.657619999999994</v>
+      </c>
+      <c r="H56" s="8">
+        <v>118.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="14">
+        <v>44712</v>
+      </c>
+      <c r="B57" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <v>48478</v>
+      </c>
+      <c r="D57">
+        <v>69</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>43.278190000000002</v>
+      </c>
+      <c r="G57">
+        <v>-97.630039999999994</v>
+      </c>
+      <c r="H57" s="7">
+        <v>126.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H58" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">

</xml_diff>